<commit_message>
update xlsx for ut10
</commit_message>
<xml_diff>
--- a/backend/utils/Ejercicios UT 10.xlsx
+++ b/backend/utils/Ejercicios UT 10.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="677">
   <si>
     <t>ID</t>
   </si>
@@ -275,19 +275,19 @@
     <t>94_136</t>
   </si>
   <si>
+    <t>ej15</t>
+  </si>
+  <si>
+    <t>BIBERONES 1</t>
+  </si>
+  <si>
+    <t>ej16</t>
+  </si>
+  <si>
+    <t>BIBERONES 2</t>
+  </si>
+  <si>
     <t>ej17</t>
-  </si>
-  <si>
-    <t>BIBERONES 1</t>
-  </si>
-  <si>
-    <t>ej18</t>
-  </si>
-  <si>
-    <t>BIBERONES 2</t>
-  </si>
-  <si>
-    <t>ej19</t>
   </si>
   <si>
     <t>BIBERONES 3</t>
@@ -2185,6 +2185,12 @@
     <t>int220</t>
   </si>
   <si>
+    <t>int221</t>
+  </si>
+  <si>
+    <t>Retirada de EPI´S</t>
+  </si>
+  <si>
     <t>Rol -------------------</t>
   </si>
   <si>
@@ -2264,7 +2270,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2310,6 +2316,11 @@
       <sz val="10.0"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="26">
@@ -2515,7 +2526,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2664,7 +2675,7 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="16" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="17" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -2676,7 +2687,7 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="3" fillId="16" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="17" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -2800,6 +2811,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
@@ -14653,9 +14667,18 @@
       <c r="E221" s="1"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="B222" s="1"/>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1"/>
+      <c r="A222" s="101" t="s">
+        <v>650</v>
+      </c>
+      <c r="B222" s="100" t="s">
+        <v>651</v>
+      </c>
+      <c r="C222" s="100">
+        <v>1.0</v>
+      </c>
+      <c r="D222" s="100" t="s">
+        <v>98</v>
+      </c>
       <c r="E222" s="1"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
@@ -19338,31 +19361,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="101">
+      <c r="A2" s="102">
         <v>0.0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="101">
+      <c r="A3" s="102">
         <v>1.0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="101">
+      <c r="A4" s="102">
         <v>2.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -19371,32 +19394,32 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="4"/>
-      <c r="B6" s="102" t="s">
-        <v>654</v>
+      <c r="B6" s="103" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="101">
+      <c r="A7" s="102">
         <v>0.0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="101">
+      <c r="A8" s="102">
         <v>1.0</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="101">
+      <c r="A9" s="102">
         <v>2.0</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -19405,32 +19428,32 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="4"/>
-      <c r="B11" s="103" t="s">
-        <v>658</v>
+      <c r="B11" s="104" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="101">
+      <c r="A12" s="102">
         <v>0.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="101">
+      <c r="A13" s="102">
         <v>1.0</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="101">
+      <c r="A14" s="102">
         <v>2.0</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -19439,40 +19462,40 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="4"/>
-      <c r="B16" s="104" t="s">
-        <v>661</v>
+      <c r="B16" s="105" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="101">
+      <c r="A17" s="102">
         <v>0.0</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="101">
+      <c r="A18" s="102">
         <v>1.0</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="101">
+      <c r="A19" s="102">
         <v>2.0</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="101">
+      <c r="A20" s="102">
         <v>3.0</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -19481,40 +19504,40 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4"/>
-      <c r="B22" s="105" t="s">
-        <v>666</v>
+      <c r="B22" s="106" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="101">
+      <c r="A23" s="102">
         <v>0.0</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="101">
+      <c r="A24" s="102">
         <v>1.0</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="101">
+      <c r="A25" s="102">
         <v>2.0</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="101">
+      <c r="A26" s="102">
         <v>3.0</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -19523,32 +19546,32 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="4"/>
-      <c r="B28" s="106" t="s">
-        <v>671</v>
+      <c r="B28" s="107" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="101">
+      <c r="A29" s="102">
         <v>0.0</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="101">
+      <c r="A30" s="102">
         <v>1.0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="101">
+      <c r="A31" s="102">
         <v>2.0</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">

</xml_diff>